<commit_message>
Began clean up the words
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F81695-C7E5-4E0F-9B14-22062C64F331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376C46FB-E5D3-445C-9E90-94F5E63486D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,7 +139,7 @@
     <t>Finished 5 small problems</t>
   </si>
   <si>
-    <t>Finished 1 small problem</t>
+    <t>Finished 1 small problem, worked on a second</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1220,7 @@
         <v>17</v>
       </c>
       <c r="C59" s="1">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>35</v>
@@ -1258,7 +1258,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>81.150000000000006</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish clean up the words
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376C46FB-E5D3-445C-9E90-94F5E63486D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C279A8E-864C-45F1-B365-90C0CC057922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>Course</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Finished 5 small problems</t>
-  </si>
-  <si>
-    <t>Finished 1 small problem, worked on a second</t>
   </si>
 </sst>
 </file>
@@ -524,19 +521,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.54296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -550,13 +547,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>44450</v>
       </c>
@@ -567,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -578,13 +575,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>44451</v>
       </c>
@@ -595,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>44452</v>
       </c>
@@ -606,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>44453</v>
       </c>
@@ -617,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>44454</v>
       </c>
@@ -631,7 +628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>44455</v>
       </c>
@@ -642,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>44456</v>
       </c>
@@ -653,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>44457</v>
       </c>
@@ -664,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -675,13 +672,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>44458</v>
       </c>
@@ -692,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>44459</v>
       </c>
@@ -703,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>44460</v>
       </c>
@@ -714,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>44461</v>
       </c>
@@ -725,7 +722,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>44462</v>
       </c>
@@ -736,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>44463</v>
       </c>
@@ -747,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>44464</v>
       </c>
@@ -761,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -772,13 +769,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>44465</v>
       </c>
@@ -789,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>44466</v>
       </c>
@@ -800,7 +797,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>44467</v>
       </c>
@@ -811,7 +808,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>44468</v>
       </c>
@@ -822,7 +819,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>44469</v>
       </c>
@@ -833,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>44470</v>
       </c>
@@ -844,7 +841,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>44471</v>
       </c>
@@ -855,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -866,13 +863,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>44472</v>
       </c>
@@ -883,7 +880,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>44473</v>
       </c>
@@ -894,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>44474</v>
       </c>
@@ -905,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>44475</v>
       </c>
@@ -919,7 +916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>44476</v>
       </c>
@@ -933,7 +930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>44477</v>
       </c>
@@ -944,7 +941,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>44478</v>
       </c>
@@ -955,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -966,7 +963,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>44479</v>
       </c>
@@ -980,7 +977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>44480</v>
       </c>
@@ -994,7 +991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>44481</v>
       </c>
@@ -1008,7 +1005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>44482</v>
       </c>
@@ -1022,7 +1019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44483</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44484</v>
       </c>
@@ -1050,7 +1047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>44485</v>
       </c>
@@ -1064,7 +1061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1075,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>44486</v>
       </c>
@@ -1089,7 +1086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>44487</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>44488</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>44489</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>44490</v>
       </c>
@@ -1145,7 +1142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>44491</v>
       </c>
@@ -1159,7 +1156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>44492</v>
       </c>
@@ -1173,7 +1170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -1184,7 +1181,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>44493</v>
       </c>
@@ -1198,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>44494</v>
       </c>
@@ -1212,7 +1209,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>44495</v>
       </c>
@@ -1220,37 +1217,37 @@
         <v>17</v>
       </c>
       <c r="C59" s="1">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>44496</v>
       </c>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>44497</v>
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>44498</v>
       </c>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>44499</v>
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="2" t="s">
         <v>12</v>
@@ -1258,16 +1255,16 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>5.25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>81.900000000000006</v>
+        <v>82.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish redo & anki for clean up the words
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C279A8E-864C-45F1-B365-90C0CC057922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB2A869-73A8-4937-9A97-CF43D937FAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,19 +521,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -547,13 +547,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>44450</v>
       </c>
@@ -564,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -575,13 +575,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>44451</v>
       </c>
@@ -592,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>44452</v>
       </c>
@@ -603,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>44453</v>
       </c>
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>44454</v>
       </c>
@@ -628,7 +628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>44455</v>
       </c>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>44456</v>
       </c>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>44457</v>
       </c>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -672,13 +672,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>44458</v>
       </c>
@@ -689,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>44459</v>
       </c>
@@ -700,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>44460</v>
       </c>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>44461</v>
       </c>
@@ -722,7 +722,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>44462</v>
       </c>
@@ -733,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>44463</v>
       </c>
@@ -744,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>44464</v>
       </c>
@@ -758,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -769,13 +769,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>44465</v>
       </c>
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>44466</v>
       </c>
@@ -797,7 +797,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>44467</v>
       </c>
@@ -808,7 +808,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>44468</v>
       </c>
@@ -819,7 +819,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>44469</v>
       </c>
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>44470</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>44471</v>
       </c>
@@ -852,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -863,13 +863,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>44472</v>
       </c>
@@ -880,7 +880,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>44473</v>
       </c>
@@ -891,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>44474</v>
       </c>
@@ -902,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>44475</v>
       </c>
@@ -916,7 +916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>44476</v>
       </c>
@@ -930,7 +930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>44477</v>
       </c>
@@ -941,7 +941,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>44478</v>
       </c>
@@ -952,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -963,7 +963,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>44479</v>
       </c>
@@ -977,7 +977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>44480</v>
       </c>
@@ -991,7 +991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>44481</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>44482</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44483</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44484</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>44485</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1072,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>44486</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>44487</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>44488</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>44489</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>44490</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>44491</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>44492</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -1181,7 +1181,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>44493</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>44494</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>44495</v>
       </c>
@@ -1217,37 +1217,37 @@
         <v>17</v>
       </c>
       <c r="C59" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>44496</v>
       </c>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>44497</v>
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>44498</v>
       </c>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>44499</v>
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2" t="s">
         <v>12</v>
@@ -1255,16 +1255,16 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>82.15</v>
+        <v>82.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganize files and find what century is that
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB2A869-73A8-4937-9A97-CF43D937FAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23FCFC0-0AE8-4FCD-930D-3CA101D29FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>Course</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Finished 5 small problems</t>
+  </si>
+  <si>
+    <t>Finished 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1230,15 @@
       <c r="A60" s="5">
         <v>44496</v>
       </c>
-      <c r="C60" s="1"/>
+      <c r="B60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -1255,7 +1266,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,7 +1275,7 @@
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>82.65</v>
+        <v>83.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish how old is Teddy
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23FCFC0-0AE8-4FCD-930D-3CA101D29FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EFD887-DC4F-41DF-B3B3-6FAF18673129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
   <si>
     <t>Course</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Finished 5 small problems</t>
-  </si>
-  <si>
-    <t>Finished 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -525,7 +522,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,10 +1231,10 @@
         <v>17</v>
       </c>
       <c r="C60" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1263,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1275,7 +1272,7 @@
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>83.15</v>
+        <v>83.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish when will i retire
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3323C09-00A2-4592-9E98-02EFFB6411D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B1699D-ECD8-4686-AEEB-7095B3003FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Course</t>
   </si>
@@ -91,9 +91,6 @@
     <t>LS95 = 14 hours</t>
   </si>
   <si>
-    <t>Finish exercises + .5 hours of cheatsheets / JS100 = 37 hours</t>
-  </si>
-  <si>
     <t>Finish Lesson 1, completed 4 small problems</t>
   </si>
   <si>
@@ -139,7 +136,16 @@
     <t>Finished 5 small problems</t>
   </si>
   <si>
-    <t>Finished 3 small problems</t>
+    <t>Finished 4 small problems</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>Finish exercises + .5 hours of cheatsheets</t>
+  </si>
+  <si>
+    <t>JS100 = 37 hours</t>
   </si>
 </sst>
 </file>
@@ -204,7 +210,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -216,6 +225,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -247,13 +259,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:D65" totalsRowCount="1" dataDxfId="8">
-  <autoFilter ref="A1:D64" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="4" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E65" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:E64" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A50C7FB5-E8D1-46A9-8CDE-3F2976E1126B}" name="Milestones" dataDxfId="5" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -522,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +546,11 @@
     <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -549,14 +563,18 @@
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>44450</v>
       </c>
@@ -566,8 +584,9 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -577,14 +596,16 @@
         <f>SUM(C3)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>44451</v>
       </c>
@@ -594,8 +615,9 @@
       <c r="C6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>44452</v>
       </c>
@@ -605,8 +627,9 @@
       <c r="C7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>44453</v>
       </c>
@@ -616,8 +639,9 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>44454</v>
       </c>
@@ -627,11 +651,11 @@
       <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>44455</v>
       </c>
@@ -641,8 +665,9 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>44456</v>
       </c>
@@ -652,8 +677,9 @@
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>44457</v>
       </c>
@@ -663,8 +689,9 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -674,14 +701,16 @@
         <f>SUM(C6:C12)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>44458</v>
       </c>
@@ -691,8 +720,9 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>44459</v>
       </c>
@@ -702,8 +732,9 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>44460</v>
       </c>
@@ -713,8 +744,9 @@
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>44461</v>
       </c>
@@ -724,8 +756,9 @@
       <c r="C18" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>44462</v>
       </c>
@@ -735,8 +768,9 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>44463</v>
       </c>
@@ -746,8 +780,9 @@
       <c r="C20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>44464</v>
       </c>
@@ -760,8 +795,9 @@
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -771,14 +807,16 @@
         <f>SUM(C15:C21)</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>44465</v>
       </c>
@@ -788,8 +826,9 @@
       <c r="C24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>44466</v>
       </c>
@@ -799,8 +838,9 @@
       <c r="C25" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>44467</v>
       </c>
@@ -810,8 +850,9 @@
       <c r="C26" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>44468</v>
       </c>
@@ -821,8 +862,9 @@
       <c r="C27" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>44469</v>
       </c>
@@ -832,8 +874,9 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>44470</v>
       </c>
@@ -843,8 +886,9 @@
       <c r="C29" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>44471</v>
       </c>
@@ -854,8 +898,9 @@
       <c r="C30" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -865,14 +910,16 @@
         <f>SUM(C24:C30)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>44472</v>
       </c>
@@ -882,8 +929,9 @@
       <c r="C33" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>44473</v>
       </c>
@@ -893,8 +941,9 @@
       <c r="C34" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>44474</v>
       </c>
@@ -904,8 +953,9 @@
       <c r="C35" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>44475</v>
       </c>
@@ -918,8 +968,9 @@
       <c r="D36" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>44476</v>
       </c>
@@ -932,8 +983,9 @@
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>44477</v>
       </c>
@@ -943,8 +995,9 @@
       <c r="C38" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>44478</v>
       </c>
@@ -954,8 +1007,9 @@
       <c r="C39" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -965,8 +1019,9 @@
         <f>SUM(C33:C39)</f>
         <v>15.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>44479</v>
       </c>
@@ -977,10 +1032,13 @@
         <v>2.5</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>44480</v>
       </c>
@@ -991,10 +1049,11 @@
         <v>3.5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>44481</v>
       </c>
@@ -1005,10 +1064,11 @@
         <v>1.25</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>44482</v>
       </c>
@@ -1019,10 +1079,11 @@
         <v>1.75</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44483</v>
       </c>
@@ -1033,10 +1094,11 @@
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44484</v>
       </c>
@@ -1047,10 +1109,11 @@
         <v>3.5</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>44485</v>
       </c>
@@ -1061,10 +1124,11 @@
         <v>1.5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1074,8 +1138,9 @@
         <f>SUM(C41:C47)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>44486</v>
       </c>
@@ -1086,10 +1151,11 @@
         <v>0.75</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>44487</v>
       </c>
@@ -1100,10 +1166,11 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>44488</v>
       </c>
@@ -1114,10 +1181,11 @@
         <v>2.15</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>44489</v>
       </c>
@@ -1128,10 +1196,11 @@
         <v>1.75</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>44490</v>
       </c>
@@ -1142,10 +1211,11 @@
         <v>1.5</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>44491</v>
       </c>
@@ -1156,10 +1226,11 @@
         <v>1.75</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>44492</v>
       </c>
@@ -1170,10 +1241,11 @@
         <v>1.75</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -1183,8 +1255,9 @@
         <f>SUM(C49:C55)</f>
         <v>10.65</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>44493</v>
       </c>
@@ -1195,10 +1268,11 @@
         <v>2.25</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>44494</v>
       </c>
@@ -1209,10 +1283,11 @@
         <v>1.75</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>44495</v>
       </c>
@@ -1223,10 +1298,11 @@
         <v>2</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>44496</v>
       </c>
@@ -1234,31 +1310,35 @@
         <v>17</v>
       </c>
       <c r="C60" s="1">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>44497</v>
       </c>
       <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>44498</v>
       </c>
       <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>44499</v>
       </c>
       <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2" t="s">
         <v>12</v>
@@ -1266,17 +1346,19 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>84.4</v>
-      </c>
+        <v>84.65</v>
+      </c>
+      <c r="E65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish 1 problem from 3.2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E34E86-59A1-4602-846A-FAED433ED9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C45D6B-B05E-4615-A0F1-73375369FA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,10 +148,10 @@
     <t>Finished 8 small problems</t>
   </si>
   <si>
-    <t>Finished 5 problems from 3.1</t>
-  </si>
-  <si>
     <t>Finished 3 small problems, 15 mins on 5 problems from 3.1</t>
+  </si>
+  <si>
+    <t>Finished 5 problems from 3.1, 1 problem from 3.2</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1334,7 @@
         <v>2.15</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1346,10 +1346,10 @@
         <v>17</v>
       </c>
       <c r="C62" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -1368,7 +1368,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>11.15</v>
+        <v>11.4</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>87.800000000000011</v>
+        <v>88.050000000000011</v>
       </c>
       <c r="E65" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Lesson 3.3 Question 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C45D6B-B05E-4615-A0F1-73375369FA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AE0EC1-C7DA-4F37-98C4-70018EB07190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,10 +148,10 @@
     <t>Finished 8 small problems</t>
   </si>
   <si>
-    <t>Finished 3 small problems, 15 mins on 5 problems from 3.1</t>
-  </si>
-  <si>
-    <t>Finished 5 problems from 3.1, 1 problem from 3.2</t>
+    <t>Finished 5 problems from 3.2, 2 problems from 3.3</t>
+  </si>
+  <si>
+    <t>Finished 3 small problems, 15 mins on 5 problems from 3.2</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1334,7 @@
         <v>2.15</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1346,10 +1346,10 @@
         <v>17</v>
       </c>
       <c r="C62" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -1368,7 +1368,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3">
         <f>SUM(C57:C63)</f>
-        <v>11.4</v>
+        <v>11.65</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="C65" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>88.050000000000011</v>
+        <v>88.300000000000011</v>
       </c>
       <c r="E65" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished 2 problems from 3.4
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20119A61-04A2-4A85-943D-A5E525E955D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3D6063-A927-4510-BA5C-1FEFF97DC10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
     <t>Anki</t>
   </si>
   <si>
-    <t>Finished 3 problems from 3.3, Anki</t>
+    <t>Finished 3 problems from 3.3, Anki, 2 problems from 3.4</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish 2 questions from 3.5
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AC66B3-C4BD-4DF7-98CB-40621B408BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78CA8EB-ACA6-4965-B11E-CC8A84BC574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Anki</t>
   </si>
   <si>
-    <t>3 problems from 3.4</t>
-  </si>
-  <si>
     <t>exercises + .5 hours of cheatsheets</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>4 small problems + further exploration</t>
+  </si>
+  <si>
+    <t>3 problems from 3.4, 2 questions from 3.5</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,7 @@
         <v>2.5</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>22</v>
@@ -1064,7 +1064,7 @@
         <v>3.5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E42" s="1"/>
     </row>
@@ -1079,7 +1079,7 @@
         <v>1.25</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E43" s="1"/>
     </row>
@@ -1094,7 +1094,7 @@
         <v>1.75</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E44" s="1"/>
     </row>
@@ -1109,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E45" s="1"/>
     </row>
@@ -1124,7 +1124,7 @@
         <v>3.5</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E46" s="1"/>
     </row>
@@ -1139,7 +1139,7 @@
         <v>1.5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E47" s="1"/>
     </row>
@@ -1181,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1196,7 +1196,7 @@
         <v>2.15</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E51" s="1"/>
     </row>
@@ -1211,7 +1211,7 @@
         <v>1.75</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E52" s="1"/>
     </row>
@@ -1256,7 +1256,7 @@
         <v>1.75</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1283,7 +1283,7 @@
         <v>2.25</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E57" s="1"/>
     </row>
@@ -1298,7 +1298,7 @@
         <v>1.75</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E58" s="1"/>
     </row>
@@ -1313,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E59" s="1"/>
     </row>
@@ -1328,7 +1328,7 @@
         <v>2.5</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -1343,7 +1343,7 @@
         <v>2.15</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1358,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -1373,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E63" s="1"/>
     </row>
@@ -1415,7 +1415,7 @@
         <v>0.5</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E66" s="1"/>
     </row>
@@ -1427,10 +1427,10 @@
         <v>17</v>
       </c>
       <c r="C67" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E67" s="1"/>
     </row>
@@ -1470,7 +1470,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3">
         <f>SUM(C65:C71)</f>
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C73" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>90.550000000000011</v>
+        <v>91.050000000000011</v>
       </c>
       <c r="E73" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 3 hard problems from 3.6
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734DEE92-638C-4BDF-944F-CA264838F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B2DA84-E5FC-4B11-845A-4D5D61CA2978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
   <si>
     <t>Course</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>8 questions from 3.5</t>
+  </si>
+  <si>
+    <t>3 questions from 3.6</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1459,15 @@
       <c r="A69" s="5">
         <v>44504</v>
       </c>
-      <c r="C69" s="1"/>
+      <c r="B69" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,7 +1492,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3">
         <f>SUM(C65:C71)</f>
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -1491,7 +1502,7 @@
       </c>
       <c r="C73" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>91.550000000000011</v>
+        <v>92.300000000000011</v>
       </c>
       <c r="E73" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish combine two lists
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C887BCA6-C03F-4B0C-87F2-F3E88EE7D229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E15F950-4DE9-44FD-8E0D-747ACD239A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
   <si>
     <t>Course</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>4 questions from 3.6; 2 small problems</t>
+  </si>
+  <si>
+    <t>3 small problems</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,10 +1481,10 @@
         <v>17</v>
       </c>
       <c r="C70" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E70" s="1"/>
     </row>
@@ -1500,7 +1503,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3">
         <f>SUM(C65:C71)</f>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -1510,7 +1513,7 @@
       </c>
       <c r="C73" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>94.550000000000011</v>
+        <v>94.800000000000011</v>
       </c>
       <c r="E73" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish multiply lists and list of digits
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B60B80C-B952-4B60-A5AD-4ACDF5E8DC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5976AB50-0C2F-4BAC-855C-2C458218095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Course</t>
   </si>
@@ -562,7 +562,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1492,15 @@
       <c r="A71" s="5">
         <v>44506</v>
       </c>
-      <c r="C71" s="1"/>
+      <c r="B71" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1503,7 +1511,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3">
         <f>SUM(C65:C71)</f>
-        <v>5.75</v>
+        <v>6.25</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -1513,7 +1521,7 @@
       </c>
       <c r="C73" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>95.050000000000011</v>
+        <v>95.550000000000011</v>
       </c>
       <c r="E73" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish basic After Midnight 1
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686EA626-6C34-4EBC-834F-B5469D32326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739D27D1-DAAA-43DB-9569-7C8794DEC86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
   <si>
     <t>Course</t>
   </si>
@@ -283,8 +283,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E73" totalsRowCount="1" dataDxfId="10">
-  <autoFilter ref="A1:E72" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E81" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:E80" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
     <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,10 +1496,10 @@
         <v>17</v>
       </c>
       <c r="C71" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E71" s="1"/>
     </row>
@@ -1511,19 +1511,80 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3">
         <f>SUM(C65:C71)</f>
-        <v>6.75</v>
+        <v>7.25</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="5">
+        <v>44507</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>44508</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>44509</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>44510</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>44511</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>44512</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>44513</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="3">
+        <f>SUM(C73:C79)</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>96.050000000000011</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>96.550000000000011</v>
+      </c>
+      <c r="E81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish After Midnight Part 1 further exploration Finish After Midnight Part 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739D27D1-DAAA-43DB-9569-7C8794DEC86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AB3D6E-E99A-4646-990F-D2951076FF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Course</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>4 small problems</t>
+  </si>
+  <si>
+    <t>only anki</t>
+  </si>
+  <si>
+    <t>further exploration and 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -561,20 +567,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -591,14 +597,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>44450</v>
       </c>
@@ -610,7 +616,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -622,14 +628,14 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>44451</v>
       </c>
@@ -641,7 +647,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>44452</v>
       </c>
@@ -653,7 +659,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>44453</v>
       </c>
@@ -665,7 +671,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>44454</v>
       </c>
@@ -679,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>44455</v>
       </c>
@@ -691,7 +697,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>44456</v>
       </c>
@@ -703,7 +709,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>44457</v>
       </c>
@@ -715,7 +721,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -727,14 +733,14 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>44458</v>
       </c>
@@ -746,7 +752,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>44459</v>
       </c>
@@ -758,7 +764,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>44460</v>
       </c>
@@ -770,7 +776,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>44461</v>
       </c>
@@ -782,7 +788,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>44462</v>
       </c>
@@ -794,7 +800,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>44463</v>
       </c>
@@ -806,7 +812,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>44464</v>
       </c>
@@ -821,7 +827,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -833,14 +839,14 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>44465</v>
       </c>
@@ -852,7 +858,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>44466</v>
       </c>
@@ -864,7 +870,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>44467</v>
       </c>
@@ -876,7 +882,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>44468</v>
       </c>
@@ -888,7 +894,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>44469</v>
       </c>
@@ -900,7 +906,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>44470</v>
       </c>
@@ -912,7 +918,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>44471</v>
       </c>
@@ -924,7 +930,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -936,14 +942,14 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>44472</v>
       </c>
@@ -955,7 +961,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>44473</v>
       </c>
@@ -967,7 +973,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>44474</v>
       </c>
@@ -979,7 +985,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>44475</v>
       </c>
@@ -994,7 +1000,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>44476</v>
       </c>
@@ -1009,7 +1015,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>44477</v>
       </c>
@@ -1021,7 +1027,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>44478</v>
       </c>
@@ -1033,7 +1039,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -1045,7 +1051,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>44479</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>44480</v>
       </c>
@@ -1077,7 +1083,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>44481</v>
       </c>
@@ -1092,7 +1098,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>44482</v>
       </c>
@@ -1107,7 +1113,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44483</v>
       </c>
@@ -1122,7 +1128,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44484</v>
       </c>
@@ -1137,7 +1143,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>44485</v>
       </c>
@@ -1152,7 +1158,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1164,7 +1170,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>44486</v>
       </c>
@@ -1179,7 +1185,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>44487</v>
       </c>
@@ -1194,7 +1200,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>44488</v>
       </c>
@@ -1209,7 +1215,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>44489</v>
       </c>
@@ -1224,7 +1230,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>44490</v>
       </c>
@@ -1239,7 +1245,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>44491</v>
       </c>
@@ -1254,7 +1260,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>44492</v>
       </c>
@@ -1269,7 +1275,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -1281,7 +1287,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>44493</v>
       </c>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>44494</v>
       </c>
@@ -1311,7 +1317,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>44495</v>
       </c>
@@ -1326,7 +1332,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>44496</v>
       </c>
@@ -1341,7 +1347,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>44497</v>
       </c>
@@ -1356,7 +1362,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>44498</v>
       </c>
@@ -1371,7 +1377,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>44499</v>
       </c>
@@ -1386,7 +1392,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="3" t="s">
         <v>12</v>
@@ -1398,7 +1404,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>44500</v>
       </c>
@@ -1413,7 +1419,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>44501</v>
       </c>
@@ -1428,7 +1434,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>44502</v>
       </c>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>44503</v>
       </c>
@@ -1458,7 +1464,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>44504</v>
       </c>
@@ -1473,7 +1479,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>44505</v>
       </c>
@@ -1488,7 +1494,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>44506</v>
       </c>
@@ -1503,7 +1509,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="3" t="s">
         <v>12</v>
@@ -1515,56 +1521,72 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>44507</v>
       </c>
-      <c r="C73" s="1"/>
+      <c r="B73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>44508</v>
       </c>
-      <c r="C74" s="1"/>
+      <c r="B74" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>44509</v>
       </c>
       <c r="C75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>44510</v>
       </c>
       <c r="C76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>44511</v>
       </c>
       <c r="C77" s="1"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>44512</v>
       </c>
       <c r="C78" s="1"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>44513</v>
       </c>
       <c r="C79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="3" t="s">
         <v>12</v>
@@ -1572,17 +1594,17 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>96.550000000000011</v>
+        <v>97.450000000000017</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish double char 1 & 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AB3D6E-E99A-4646-990F-D2951076FF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C4414-D212-497A-8788-9C6B2379266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
     <t>only anki</t>
   </si>
   <si>
-    <t>further exploration and 1 small problem</t>
+    <t>further exploration and 3 small problems</t>
   </si>
 </sst>
 </file>
@@ -567,20 +567,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -597,14 +597,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>44450</v>
       </c>
@@ -616,7 +616,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
@@ -628,14 +628,14 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>44451</v>
       </c>
@@ -647,7 +647,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>44452</v>
       </c>
@@ -659,7 +659,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>44453</v>
       </c>
@@ -671,7 +671,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>44454</v>
       </c>
@@ -685,7 +685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>44455</v>
       </c>
@@ -697,7 +697,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>44456</v>
       </c>
@@ -709,7 +709,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>44457</v>
       </c>
@@ -721,7 +721,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -733,14 +733,14 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>44458</v>
       </c>
@@ -752,7 +752,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>44459</v>
       </c>
@@ -764,7 +764,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>44460</v>
       </c>
@@ -776,7 +776,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>44461</v>
       </c>
@@ -788,7 +788,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>44462</v>
       </c>
@@ -800,7 +800,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>44463</v>
       </c>
@@ -812,7 +812,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>44464</v>
       </c>
@@ -827,7 +827,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -839,14 +839,14 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>44465</v>
       </c>
@@ -858,7 +858,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>44466</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>44467</v>
       </c>
@@ -882,7 +882,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>44468</v>
       </c>
@@ -894,7 +894,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>44469</v>
       </c>
@@ -906,7 +906,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>44470</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>44471</v>
       </c>
@@ -930,7 +930,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -942,14 +942,14 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>44472</v>
       </c>
@@ -961,7 +961,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>44473</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>44474</v>
       </c>
@@ -985,7 +985,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>44475</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>44476</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>44477</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>44478</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>44479</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>44480</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>44481</v>
       </c>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>44482</v>
       </c>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44483</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44484</v>
       </c>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>44485</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>44486</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>44487</v>
       </c>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>44488</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>44489</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>44490</v>
       </c>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>44491</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>44492</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>44493</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>44494</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>44495</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>44496</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>44497</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>44498</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>44499</v>
       </c>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="3" t="s">
         <v>12</v>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>44500</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>44501</v>
       </c>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>44502</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>44503</v>
       </c>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>44504</v>
       </c>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>44505</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>44506</v>
       </c>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="3" t="s">
         <v>12</v>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>44507</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>44508</v>
       </c>
@@ -1544,49 +1544,49 @@
         <v>17</v>
       </c>
       <c r="C74" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>44509</v>
       </c>
       <c r="C75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>44510</v>
       </c>
       <c r="C76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>44511</v>
       </c>
       <c r="C77" s="1"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>44512</v>
       </c>
       <c r="C78" s="1"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>44513</v>
       </c>
       <c r="C79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="3" t="s">
         <v>12</v>
@@ -1594,17 +1594,17 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>97.450000000000017</v>
+        <v>97.950000000000017</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish always return negative, get the middle char, reverse number
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C4414-D212-497A-8788-9C6B2379266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F7A1EE-4B5B-4E57-8C55-A3B468103A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,7 +175,7 @@
     <t>only anki</t>
   </si>
   <si>
-    <t>further exploration and 3 small problems</t>
+    <t>further exploration and 5 small problems</t>
   </si>
 </sst>
 </file>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1544,7 @@
         <v>17</v>
       </c>
       <c r="C74" s="1">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>47</v>
@@ -1594,7 +1594,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>97.950000000000017</v>
+        <v>98.450000000000017</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish counting up, name swapping, sequence count
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F7A1EE-4B5B-4E57-8C55-A3B468103A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152AEDC5-109D-40A5-80E4-A13B98A6E7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
   <si>
     <t>Course</t>
   </si>
@@ -175,7 +175,10 @@
     <t>only anki</t>
   </si>
   <si>
-    <t>further exploration and 5 small problems</t>
+    <t>further exploration and 9 small problems</t>
+  </si>
+  <si>
+    <t>Start Lesson 4</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1532,7 @@
         <v>17</v>
       </c>
       <c r="C73" s="1">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>46</v>
@@ -1544,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="C74" s="1">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>47</v>
@@ -1556,6 +1559,9 @@
         <v>44509</v>
       </c>
       <c r="C75" s="1"/>
+      <c r="D75" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,7 +1600,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1604,7 +1610,7 @@
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>98.450000000000017</v>
+        <v>99.050000000000011</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 4.6 through Data Structures
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110ADF57-0DC5-4D7D-B024-9DF1ED5954BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42382F15-8DF0-4666-BE56-06F36ACA82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
   <si>
     <t>Course</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Lesson 4.3, 4.4, 4.5</t>
+  </si>
+  <si>
+    <t>Lesson 4.6: Problem through Data Structures</t>
   </si>
 </sst>
 </file>
@@ -251,6 +254,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -263,13 +269,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -298,11 +301,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E81" totalsRowCount="1" dataDxfId="10">
   <autoFilter ref="A1:E80" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A50C7FB5-E8D1-46A9-8CDE-3F2976E1126B}" name="Milestones" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A50C7FB5-E8D1-46A9-8CDE-3F2976E1126B}" name="Milestones" dataDxfId="5" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1594,15 @@
       <c r="A77" s="5">
         <v>44511</v>
       </c>
-      <c r="C77" s="1"/>
+      <c r="B77" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,7 +1627,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>5.25</v>
+        <v>5.75</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1626,7 +1637,7 @@
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>101.80000000000001</v>
+        <v>102.30000000000001</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 4.6 through Algorithms
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42382F15-8DF0-4666-BE56-06F36ACA82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2571673E-6F39-43FB-9494-DBD769A77EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>Lesson 4.3, 4.4, 4.5</t>
   </si>
   <si>
-    <t>Lesson 4.6: Problem through Data Structures</t>
+    <t>Lesson 4.6: Problem through Algorithms</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1598,7 @@
         <v>17</v>
       </c>
       <c r="C77" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>50</v>
@@ -1627,7 +1627,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>5.75</v>
+        <v>6</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="C81" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>102.30000000000001</v>
+        <v>102.55000000000001</v>
       </c>
       <c r="E81" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Lesson 4 Quiz
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480D61A0-131C-47B9-9B69-EA6CEE99EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67413E1-804F-4C17-BA21-2E56AB462F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
     <t>4.6 Implementation, 4.7, 4.8 forEach</t>
   </si>
   <si>
-    <t>Finish 4.8, 4.9, 4.10, 4.11</t>
+    <t>Finish 4.8, 4.9, 4.10, 4.11, quiz</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1634,7 @@
         <v>17</v>
       </c>
       <c r="C79" s="1">
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>52</v>
@@ -1649,7 +1649,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>9.75</v>
+        <v>11</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>106.30000000000001</v>
+        <v>107.55000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish reverse it 1
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67413E1-804F-4C17-BA21-2E56AB462F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF74B6C-5AF2-42E8-A9C0-485DF2104C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>Course</t>
   </si>
@@ -190,7 +190,10 @@
     <t>4.6 Implementation, 4.7, 4.8 forEach</t>
   </si>
   <si>
-    <t>Finish 4.8, 4.9, 4.10, 4.11, quiz</t>
+    <t>Finish 4.8, 4.9, 4.10, 4.11, quiz, 1 small problem</t>
+  </si>
+  <si>
+    <t>Finish Lesson 4</t>
   </si>
 </sst>
 </file>
@@ -1634,12 +1637,14 @@
         <v>17</v>
       </c>
       <c r="C79" s="1">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E79" s="1"/>
+      <c r="E79" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
@@ -1649,7 +1654,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3">
         <f>SUM(C73:C79)</f>
-        <v>11</v>
+        <v>11.25</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -1720,7 +1725,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>107.55000000000001</v>
+        <v>107.80000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish reverse it 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF74B6C-5AF2-42E8-A9C0-485DF2104C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86A4575-7EB3-4F0A-8110-11BAC88125BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>Course</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Finish Lesson 4</t>
+  </si>
+  <si>
+    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1665,15 @@
       <c r="A81" s="5">
         <v>44514</v>
       </c>
-      <c r="C81" s="1"/>
+      <c r="B81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1715,7 +1726,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1725,7 +1736,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>107.80000000000001</v>
+        <v>108.30000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish sum of digits
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7A51BD-3576-4BA1-B0CD-E981530166F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFDAEE-0B49-49A5-99EB-B22FF8458C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <t>Finish Lesson 4</t>
   </si>
   <si>
-    <t>Finish 3 small problems</t>
+    <t>Finish 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1669,7 @@
         <v>17</v>
       </c>
       <c r="C81" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>54</v>
@@ -1726,7 +1726,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>109.30000000000001</v>
+        <v>109.80000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish multiply all pairs and leading substrings
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB2837D-23FC-4AFF-9D96-216479216ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6990B2B8-459D-4F78-80DE-5F96F448BC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="56">
   <si>
     <t>Course</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Finish 5 small problems</t>
+  </si>
+  <si>
+    <t>Finish 2 small problems</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1683,15 @@
       <c r="A82" s="5">
         <v>44515</v>
       </c>
-      <c r="C82" s="1"/>
+      <c r="B82" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1726,7 +1737,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1736,7 +1747,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>110.30000000000001</v>
+        <v>111.05000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish further exploration of leading substrings
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6990B2B8-459D-4F78-80DE-5F96F448BC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF66CF3-106E-4323-99A2-A691E7BFDBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1687,7 @@
         <v>17</v>
       </c>
       <c r="C82" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>55</v>
@@ -1737,7 +1737,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>111.05000000000001</v>
+        <v>111.30000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish sum of sums
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA95D414-3614-44F0-9FFD-AEAEA1335B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C08035-99E1-476F-910A-76BBC1E0607F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Course</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Finish 2 small problems</t>
+  </si>
+  <si>
+    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1716,15 @@
       <c r="A84" s="5">
         <v>44517</v>
       </c>
-      <c r="C84" s="1"/>
+      <c r="B84" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,7 +1756,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1755,7 +1766,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>112.05000000000001</v>
+        <v>112.55000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Inventory item transactions & availability
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE3D6A-CB3D-4BC9-9EC9-5E932D414A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE7DD90-5F27-4614-81F5-27F0373A482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Course</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Finish 2 small problems</t>
+  </si>
+  <si>
+    <t>Finish 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,10 +1720,10 @@
         <v>17</v>
       </c>
       <c r="C84" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E84" s="1"/>
     </row>
@@ -1753,7 +1756,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1763,7 +1766,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>112.80000000000001</v>
+        <v>113.30000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish delete vowels and uppercase check
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE7DD90-5F27-4614-81F5-27F0373A482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF9C587-0607-4006-8DA5-9738FAE2859F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,7 +202,7 @@
     <t>Finish 2 small problems</t>
   </si>
   <si>
-    <t>Finish 4 small problems</t>
+    <t>Finish 6 small problems</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1720,7 @@
         <v>17</v>
       </c>
       <c r="C84" s="1">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>56</v>
@@ -1756,7 +1756,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>113.30000000000001</v>
+        <v>113.55000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish capitalize_words, staggered_caps_1, staggered_caps_2, swap_case
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83676067-0829-467F-8757-B3A1A8EB0DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65E482-D66B-4C24-A9BD-41B3B73A9E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
   <si>
     <t>Course</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Finish 7 small problems</t>
+  </si>
+  <si>
+    <t>Finish 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1734,15 @@
       <c r="A85" s="5">
         <v>44518</v>
       </c>
-      <c r="C85" s="1"/>
+      <c r="B85" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,7 +1767,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1766,7 +1777,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>113.80000000000001</v>
+        <v>114.80000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish how long are you
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65E482-D66B-4C24-A9BD-41B3B73A9E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C8C983-1FFB-46F7-A31E-0CA0B6013003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
   <si>
     <t>Course</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>Finish 7 small problems</t>
-  </si>
-  <si>
-    <t>Finish 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,10 +1735,10 @@
         <v>17</v>
       </c>
       <c r="C85" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -1767,7 +1764,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>7</v>
+        <v>7.25</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1777,7 +1774,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>114.80000000000001</v>
+        <v>115.05000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish search word 1 & 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C8C983-1FFB-46F7-A31E-0CA0B6013003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783EE67E-AAC6-4CD2-B9BA-E839248375E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Course</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Finish 7 small problems</t>
+  </si>
+  <si>
+    <t>begin Lesson 5</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,10 +1738,10 @@
         <v>17</v>
       </c>
       <c r="C85" s="1">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -1746,8 +1749,13 @@
       <c r="A86" s="5">
         <v>44519</v>
       </c>
+      <c r="B86" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C86" s="1"/>
-      <c r="E86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
@@ -1764,7 +1772,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>7.25</v>
+        <v>7.75</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1774,7 +1782,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>115.05000000000001</v>
+        <v>115.55000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 5.4 through Example 3
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2B6BB1-565D-4FD3-B627-63008955500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC4726-D5CE-43F6-BE35-E51C7EE821A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
     <t>Finish 7 small problems, Finish 5.1-5.2</t>
   </si>
   <si>
-    <t>Finish 5.3</t>
+    <t>Finish 5.3, started 5.4 through Example 3</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1761,7 @@
         <v>17</v>
       </c>
       <c r="C86" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>59</v>
@@ -1783,7 +1783,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>116.30000000000001</v>
+        <v>116.80000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 5.4 Example 4
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC4726-D5CE-43F6-BE35-E51C7EE821A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E944547C-BAA6-4948-AF50-DF7E06263F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
     <t>Finish 7 small problems, Finish 5.1-5.2</t>
   </si>
   <si>
-    <t>Finish 5.3, started 5.4 through Example 3</t>
+    <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1761,7 @@
         <v>17</v>
       </c>
       <c r="C86" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>59</v>
@@ -1783,7 +1783,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>9</v>
+        <v>9.25</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="C89" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>116.80000000000001</v>
+        <v>117.05000000000001</v>
       </c>
       <c r="E89" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 5.5 through pp 4
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C66678-C360-4D57-823C-8360D751CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D245292-794C-4CAC-8470-AA1248CC7AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4</t>
+    <t>Finish 5.4, 5.5 practice problems 1-4</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>117.80000000000001</v>
+        <v>118.30000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 3 more practice problems
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D245292-794C-4CAC-8470-AA1248CC7AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F42D94-4AFD-4CD6-86A6-D2AC802759F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4, 5.5 practice problems 1-4</t>
+    <t>Finish 5.4, 5.5 practice problems 1-7</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>118.30000000000001</v>
+        <v>118.80000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Practice Problems 8, 9
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F42D94-4AFD-4CD6-86A6-D2AC802759F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D291653-DCBF-43EF-BC98-06305C841728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4, 5.5 practice problems 1-7</t>
+    <t>Finish 5.4, 5.5 practice problems 1-9</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>118.80000000000001</v>
+        <v>119.30000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Practice Problems 10, 11
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D291653-DCBF-43EF-BC98-06305C841728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDDB8D8-E151-466D-991D-6D56425AE13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4, 5.5 practice problems 1-9</t>
+    <t>Finish 5.4, 5.5 practice problems 1-11</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>119.30000000000001</v>
+        <v>119.80000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 5.5 pp 12 & 13
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDDB8D8-E151-466D-991D-6D56425AE13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB4EDD7-9872-4513-AF38-5C34727845A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4, 5.5 practice problems 1-11</t>
+    <t>Finish 5.4, 5.5 practice problems 1-13</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>119.80000000000001</v>
+        <v>120.30000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish 5.5 pp 14-17
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB4EDD7-9872-4513-AF38-5C34727845A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD34DCB-237D-4E0B-9A60-579989593D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <t>Finish 5.3, started 5.4 through Example 4</t>
   </si>
   <si>
-    <t>Finish 5.4, 5.5 practice problems 1-13</t>
+    <t>Finish 5.4, 5.5 practice problems 1-17</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="C87" s="1">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>60</v>
@@ -1794,7 +1794,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3">
         <f>SUM(C81:C87)</f>
-        <v>12.5</v>
+        <v>13.25</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>120.30000000000001</v>
+        <v>121.05000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish Lesson 5 Quiz
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD34DCB-237D-4E0B-9A60-579989593D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032A12C-783D-4E8C-8C5F-1178E0F1E8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Course</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Finish 5.4, 5.5 practice problems 1-17</t>
+  </si>
+  <si>
+    <t>Finish Lesson 5</t>
+  </si>
+  <si>
+    <t>Finish Lesson 5 Quiz</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,8 +1808,18 @@
       <c r="A89" s="5">
         <v>44521</v>
       </c>
-      <c r="C89" s="1"/>
-      <c r="E89" s="1"/>
+      <c r="B89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
@@ -1855,7 +1871,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1865,7 +1881,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>121.05000000000001</v>
+        <v>121.55000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish rotation 1 & 2
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032A12C-783D-4E8C-8C5F-1178E0F1E8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA68E489-2C91-4773-AE8C-C98055A238F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,7 +220,7 @@
     <t>Finish Lesson 5</t>
   </si>
   <si>
-    <t>Finish Lesson 5 Quiz</t>
+    <t>Finish Lesson 5 Quiz, 2 small problems</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1812,7 @@
         <v>17</v>
       </c>
       <c r="C89" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>62</v>
@@ -1871,7 +1871,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>121.55000000000001</v>
+        <v>122.05000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish stack machine interpretation
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA68E489-2C91-4773-AE8C-C98055A238F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FA30E4-1F42-42F4-8E78-9A457544EB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,7 +220,7 @@
     <t>Finish Lesson 5</t>
   </si>
   <si>
-    <t>Finish Lesson 5 Quiz, 2 small problems</t>
+    <t>Finish Lesson 5 Quiz, 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1812,7 @@
         <v>17</v>
       </c>
       <c r="C89" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>62</v>
@@ -1871,7 +1871,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>122.05000000000001</v>
+        <v>123.05000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish word to digit
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FA30E4-1F42-42F4-8E78-9A457544EB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF54EC7-EE54-4116-BCD7-1075A035F057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
   <si>
     <t>Course</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
+  </si>
+  <si>
+    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,7 +1828,15 @@
       <c r="A90" s="5">
         <v>44522</v>
       </c>
-      <c r="C90" s="1"/>
+      <c r="B90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1871,7 +1882,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1881,7 +1892,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>123.05000000000001</v>
+        <v>123.80000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish fibonacci numbers recursion
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF54EC7-EE54-4116-BCD7-1075A035F057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2AB4DB-CE3B-4D08-A624-7A480D680693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
   <si>
     <t>Course</t>
   </si>
@@ -221,9 +221,6 @@
   </si>
   <si>
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
-  </si>
-  <si>
-    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -1832,10 +1829,10 @@
         <v>17</v>
       </c>
       <c r="C90" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E90" s="1"/>
     </row>
@@ -1882,7 +1879,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1892,7 +1889,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>123.80000000000001</v>
+        <v>124.05000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish fibonacci procedural and memoization
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2AB4DB-CE3B-4D08-A624-7A480D680693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34942ACF-DF0B-40A5-ABC3-08D7DB932ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
   <si>
     <t>Course</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
+  </si>
+  <si>
+    <t>Finish 4 small problems</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,10 +1832,10 @@
         <v>17</v>
       </c>
       <c r="C90" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E90" s="1"/>
     </row>
@@ -1879,7 +1882,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1889,7 +1892,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>124.05000000000001</v>
+        <v>124.55000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish sum square - square sum
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF15E20A-7626-4EE9-B7BE-AC88EE705F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E40C26-3AC7-4FC4-A600-6604E5E480C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
   </si>
   <si>
-    <t>Finish 2 small problems, fixed what century</t>
+    <t>Finish 3 small problems, fixed what century</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1862,7 @@
         <v>17</v>
       </c>
       <c r="C92" s="1">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>63</v>
@@ -1898,7 +1898,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>127.30000000000001</v>
+        <v>127.55000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
First version of bubble sort
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E40C26-3AC7-4FC4-A600-6604E5E480C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ADB8E9-F3FB-484F-9C1A-EE6B8F40F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
   </si>
   <si>
-    <t>Finish 3 small problems, fixed what century</t>
+    <t>Finish 4 small problems, fixed what century</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1862,7 @@
         <v>17</v>
       </c>
       <c r="C92" s="1">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>63</v>
@@ -1898,7 +1898,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>127.55000000000001</v>
+        <v>127.80000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish revising bubble sort & first version of longest sentence
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ADB8E9-F3FB-484F-9C1A-EE6B8F40F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2103BC47-CF26-4323-808A-49D8EF3F6773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
     <t>Finish Lesson 5 Quiz, 4 small problems</t>
   </si>
   <si>
-    <t>Finish 4 small problems, fixed what century</t>
+    <t>Finish 5 small problems, fixed what century</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1862,7 @@
         <v>17</v>
       </c>
       <c r="C92" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>63</v>
@@ -1898,7 +1898,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>6.75</v>
+        <v>7.25</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>127.80000000000001</v>
+        <v>128.30000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish longest sentence further exploration
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2103BC47-CF26-4323-808A-49D8EF3F6773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD640104-0C70-4C1B-B0C9-4F2B5EBC8FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1862,7 @@
         <v>17</v>
       </c>
       <c r="C92" s="1">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>63</v>
@@ -1898,7 +1898,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>7.25</v>
+        <v>7.5</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>128.30000000000001</v>
+        <v>128.55000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish diamond and hollow diamond
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B177F2-5DD8-4EA7-ACD5-2DC96249CC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB3853F-2A90-4288-960E-39CFD6ECA77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>Course</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Finish 6 small problems, fixed what century</t>
+  </si>
+  <si>
+    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1876,15 @@
       <c r="A93" s="5">
         <v>44525</v>
       </c>
-      <c r="C93" s="1"/>
+      <c r="B93" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1909,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1908,7 +1919,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>129.05000000000001</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish now i know my abcs
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB3853F-2A90-4288-960E-39CFD6ECA77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA629EB9-9D47-4BC5-AC0D-F55C86ACACAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="64">
   <si>
     <t>Course</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Finish 6 small problems, fixed what century</t>
-  </si>
-  <si>
-    <t>Finish 1 small problem</t>
   </si>
 </sst>
 </file>
@@ -619,7 +616,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,10 +1877,10 @@
         <v>17</v>
       </c>
       <c r="C93" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E93" s="1"/>
     </row>
@@ -1909,7 +1906,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3">
         <f>SUM(C89:C95)</f>
-        <v>8.75</v>
+        <v>9.25</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -1919,7 +1916,7 @@
       </c>
       <c r="C97" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>129.80000000000001</v>
+        <v>130.30000000000001</v>
       </c>
       <c r="E97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Mostly finish 6.8 Keep Score
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3823752-65A4-45CF-9DEF-3BC6223932FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E845A1-5ADB-4A23-AC4C-F5D0B5861735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="76">
   <si>
     <t>Course</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Finish 6.6-7, 6.8 joinOr</t>
+  </si>
+  <si>
+    <t>Finish 6.8 Keep Score</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2052,15 @@
       <c r="A106" s="5">
         <v>44529</v>
       </c>
-      <c r="C106" s="1"/>
+      <c r="B106" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,7 +2106,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2105,7 +2116,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>134.55000000000001</v>
+        <v>135.55000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish 6.8 keep score
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E845A1-5ADB-4A23-AC4C-F5D0B5861735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C7695-CE48-4923-9BAA-40478CC903CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2056,7 @@
         <v>17</v>
       </c>
       <c r="C106" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>75</v>
@@ -2106,7 +2106,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>135.55000000000001</v>
+        <v>135.80000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finish computer AI defense
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C7695-CE48-4923-9BAA-40478CC903CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6DB069-B14E-4960-9548-1CCF02D02624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
     <t>Finish 6.6-7, 6.8 joinOr</t>
   </si>
   <si>
-    <t>Finish 6.8 Keep Score</t>
+    <t>Finish 6.8 Keep Score, Defense</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2056,7 @@
         <v>17</v>
       </c>
       <c r="C106" s="1">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>75</v>
@@ -2106,7 +2106,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>135.80000000000001</v>
+        <v>136.55000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish basic offensive ai
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6DB069-B14E-4960-9548-1CCF02D02624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2AC4AA-C138-4C0D-AA30-4EC21A0E2F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
     <t>Finish 6.6-7, 6.8 joinOr</t>
   </si>
   <si>
-    <t>Finish 6.8 Keep Score, Defense</t>
+    <t>Finish 6.8 Keep Score, Defense, offense</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2056,7 @@
         <v>17</v>
       </c>
       <c r="C106" s="1">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>75</v>
@@ -2106,7 +2106,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>136.55000000000001</v>
+        <v>136.80000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish middle square first for ai
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2026000C-ABD4-40D3-8AFA-8BACD588B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE29E8F1-0CF5-41D1-9A3F-D4B53D7746DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,7 +262,7 @@
     <t>Finish 6.8 Keep Score, Defense, offense</t>
   </si>
   <si>
-    <t>Finish 6.8 consolidate AI</t>
+    <t>Finish 6.8 consolidate AI, middle square</t>
   </si>
 </sst>
 </file>
@@ -655,7 +655,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2074,7 @@
         <v>17</v>
       </c>
       <c r="C107" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>76</v>
@@ -2117,7 +2117,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>137.30000000000001</v>
+        <v>137.55000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
add first mover functionality
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE29E8F1-0CF5-41D1-9A3F-D4B53D7746DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9B1348-78A1-4575-823A-2ED83F8745C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,7 +262,7 @@
     <t>Finish 6.8 Keep Score, Defense, offense</t>
   </si>
   <si>
-    <t>Finish 6.8 consolidate AI, middle square</t>
+    <t>Finish 6.8 consolidate AI, middle square, add first mover</t>
   </si>
 </sst>
 </file>
@@ -2074,7 +2074,7 @@
         <v>17</v>
       </c>
       <c r="C107" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>76</v>
@@ -2117,7 +2117,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>137.55000000000001</v>
+        <v>137.80000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
add chooseSquare and alternatePlayer
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9B1348-78A1-4575-823A-2ED83F8745C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B8CFF0-0F90-4993-8DA1-A01B83943B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
   <si>
     <t>Course</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Finish 6.8 consolidate AI, middle square, add first mover</t>
+  </si>
+  <si>
+    <t>6.8 chooseSquare, alternatePlayer</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2088,15 @@
       <c r="A108" s="5">
         <v>44531</v>
       </c>
-      <c r="C108" s="1"/>
+      <c r="B108" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2117,7 +2128,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>4.75</v>
+        <v>5.25</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2127,7 +2138,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>137.80000000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
add choose who plays first
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B8CFF0-0F90-4993-8DA1-A01B83943B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA09A5A-EFFF-4C1F-9E99-09584668C3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
     <t>Finish 6.8 consolidate AI, middle square, add first mover</t>
   </si>
   <si>
-    <t>6.8 chooseSquare, alternatePlayer</t>
+    <t>6.8 chooseSquare, alternatePlayer, choose firstPlayer</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,7 +2092,7 @@
         <v>17</v>
       </c>
       <c r="C108" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>77</v>
@@ -2128,7 +2128,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>5.25</v>
+        <v>5.75</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>138.30000000000001</v>
+        <v>138.80000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
tidy up tic tac toe
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB882A5B-6E8F-495E-915E-F8385490B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E0DAC1-79FD-4AC9-AB0E-9502B38435B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,7 +2110,7 @@
         <v>17</v>
       </c>
       <c r="C109" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>78</v>
@@ -2139,7 +2139,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>139.30000000000001</v>
+        <v>139.55000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
hands object, format hands
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3985E422-3DD1-4D77-BBB3-8A51E66B40A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03712E39-F98B-4945-9967-8835EBD71207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
   <si>
     <t>Course</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>6.9 initialize deck, deal cards</t>
+  </si>
+  <si>
+    <t>6.9 hands object, format hands</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,7 +2142,15 @@
       <c r="A111" s="5">
         <v>44534</v>
       </c>
-      <c r="C111" s="1"/>
+      <c r="B111" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2150,7 +2161,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3">
         <f>SUM(C105:C111)</f>
-        <v>7.5</v>
+        <v>8.75</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2160,7 +2171,7 @@
       </c>
       <c r="C113" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>140.55000000000001</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="E113" s="2"/>
     </row>

</xml_diff>

<commit_message>
convert data to one cards object, displayHands function
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03712E39-F98B-4945-9967-8835EBD71207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B63F7-19E8-4014-B588-FFA0E782BEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
   <si>
     <t>Course</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>6.9 hands object, format hands</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>6.9 convert data to one cards object, displayHands function</t>
   </si>
 </sst>
 </file>
@@ -388,8 +394,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E113" totalsRowCount="1" dataDxfId="10">
-  <autoFilter ref="A1:E112" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E122" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:E121" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
     <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
@@ -664,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,14 +2172,90 @@
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5">
+        <v>44535</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="5">
+        <v>44536</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
+        <v>44537</v>
+      </c>
+      <c r="C116" s="1"/>
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>44538</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5">
+        <v>44539</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="5">
+        <v>44540</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <v>44541</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="3">
+        <f>SUM(C114:C120)</f>
+        <v>1</v>
+      </c>
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>141.80000000000001</v>
-      </c>
-      <c r="E113" s="2"/>
+        <v>142.80000000000001</v>
+      </c>
+      <c r="E122" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish playerMove, add game loop
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3A847F-7E14-4D77-8A9B-3D90A3FDDBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8CF823-27F9-464E-916D-0FB63E03E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
   <si>
     <t>Course</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>6.9 convert data to one cards object, displayHands function, calculateScore, getMaxScore, getWinners, start playerMove</t>
+  </si>
+  <si>
+    <t>6.9 added game loop, finish playerMove</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2205,15 @@
       <c r="A115" s="5">
         <v>44536</v>
       </c>
-      <c r="C115" s="1"/>
+      <c r="B115" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2248,7 +2259,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2258,7 +2269,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>145.05000000000001</v>
+        <v>145.80000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
start bonus features after constants
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FCC5F9-F62E-4F26-ABAD-EB7ABF5AB5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29151CB3-7E60-4BDB-8B05-ED080AFBFD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2227,7 +2227,7 @@
         <v>17</v>
       </c>
       <c r="C116" s="1">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>85</v>
@@ -2270,7 +2270,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>7.75</v>
+        <v>8.25</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>149.55000000000001</v>
+        <v>150.05000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add best to five, tidied up logic
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29151CB3-7E60-4BDB-8B05-ED080AFBFD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C213482-3413-4C01-9DE7-90FFE90C18E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
   <si>
     <t>Course</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Finish 6.9-11</t>
+  </si>
+  <si>
+    <t>Add best to five, tidied up logic</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,7 +2241,15 @@
       <c r="A117" s="5">
         <v>44538</v>
       </c>
-      <c r="C117" s="1"/>
+      <c r="B117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117" s="1">
+        <v>2</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2270,7 +2281,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2280,7 +2291,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>150.05000000000001</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish best of five, proper verb tense
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C213482-3413-4C01-9DE7-90FFE90C18E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE07CA-A37C-406F-97BD-A467283B3ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -685,7 +685,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2245,7 @@
         <v>17</v>
       </c>
       <c r="C117" s="1">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>86</v>
@@ -2281,7 +2281,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>10.25</v>
+        <v>10.5</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>152.05000000000001</v>
+        <v>152.30000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
fix PLAYERS const use, streamline questions
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE07CA-A37C-406F-97BD-A467283B3ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D4EDC5-4628-4FF1-BF17-15DB22D1148E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2245,7 +2245,7 @@
         <v>17</v>
       </c>
       <c r="C117" s="1">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>86</v>
@@ -2281,7 +2281,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>10.5</v>
+        <v>10.75</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>152.30000000000001</v>
+        <v>152.55000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
reorganize js_109 prep materials
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F492B2-DE1E-4AD6-BA2F-843A9895A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D562164-8DB9-45E1-8198-85C1BEB6A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,10 +295,10 @@
     <t>Add best to five, tidied up logic</t>
   </si>
   <si>
-    <t>6.12 features for their version, finish quiz</t>
-  </si>
-  <si>
     <t>Finish Lesson 6 / JS101 except for 18 small problems</t>
+  </si>
+  <si>
+    <t>6.12 features for their version, finish quiz, 2 codewars</t>
   </si>
 </sst>
 </file>
@@ -691,7 +691,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,13 +2266,13 @@
         <v>17</v>
       </c>
       <c r="C118" s="1">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="D118" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>12.75</v>
+        <v>13</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>154.55000000000001</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish two small problems
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D562164-8DB9-45E1-8198-85C1BEB6A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64976C5B-D115-4617-8B54-F0BC7BFDD8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
   <si>
     <t>Course</t>
   </si>
@@ -691,7 +691,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2279,15 @@
       <c r="A119" s="5">
         <v>44540</v>
       </c>
-      <c r="C119" s="1"/>
+      <c r="B119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,7 +2305,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2307,7 +2315,7 @@
       </c>
       <c r="C122" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>154.80000000000001</v>
+        <v>155.80000000000001</v>
       </c>
       <c r="E122" s="2"/>
     </row>

</xml_diff>

<commit_message>
finish 3 small problems
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64976C5B-D115-4617-8B54-F0BC7BFDD8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6976FFC-EBAC-4AC4-93F8-FB1275682E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="91">
   <si>
     <t>Course</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>6.12 features for their version, finish quiz, 2 codewars</t>
+  </si>
+  <si>
+    <t>Finish 3 small problems</t>
+  </si>
+  <si>
+    <t>Week 15</t>
   </si>
 </sst>
 </file>
@@ -412,8 +418,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E122" totalsRowCount="1" dataDxfId="10">
-  <autoFilter ref="A1:E121" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E131" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:E130" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
     <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
@@ -688,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,7 +2300,15 @@
       <c r="A120" s="5">
         <v>44541</v>
       </c>
-      <c r="C120" s="1"/>
+      <c r="B120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2305,19 +2319,87 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3">
         <f>SUM(C114:C120)</f>
-        <v>14</v>
+        <v>14.75</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C122" s="1"/>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5">
+        <v>44542</v>
+      </c>
+      <c r="C123" s="1"/>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <v>44543</v>
+      </c>
+      <c r="C124" s="1"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5">
+        <v>44544</v>
+      </c>
+      <c r="C125" s="1"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5">
+        <v>44545</v>
+      </c>
+      <c r="C126" s="1"/>
+      <c r="E126" s="1"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="5">
+        <v>44546</v>
+      </c>
+      <c r="C127" s="1"/>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
+        <v>44547</v>
+      </c>
+      <c r="C128" s="1"/>
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5">
+        <v>44548</v>
+      </c>
+      <c r="C129" s="1"/>
+      <c r="E129" s="1"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" s="1"/>
+      <c r="D130" s="3">
+        <f>SUM(C123:C129)</f>
+        <v>0</v>
+      </c>
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C131" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>155.80000000000001</v>
-      </c>
-      <c r="E122" s="2"/>
+        <v>156.55000000000001</v>
+      </c>
+      <c r="E131" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish 2 small problems
</commit_message>
<xml_diff>
--- a/time_log.xlsx
+++ b/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csommerlatte\js_101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63697949-5645-4A9F-8389-42E18056C96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E76049-F6EC-452F-B292-C95030E0EB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="92">
   <si>
     <t>Course</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Week 15</t>
+  </si>
+  <si>
+    <t>Finish debugging problems</t>
   </si>
 </sst>
 </file>
@@ -377,9 +380,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -387,6 +387,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -421,11 +424,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}" name="Table1" displayName="Table1" ref="A1:E131" totalsRowCount="1" dataDxfId="10">
   <autoFilter ref="A1:E130" xr:uid="{7A23BCA4-EF32-4A57-86A1-09542BE5149E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="6" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{A50C7FB5-E8D1-46A9-8CDE-3F2976E1126B}" name="Milestones" dataDxfId="5" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{46AA6834-7F30-4EFB-AC59-35B61B1FEF32}" name="Date" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{4C7D6A36-89D8-486B-A39E-A08E20E50BBB}" name="Course" dataDxfId="8" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{863655C5-5FB9-4AA1-AF47-BC5B52735F62}" name="Hours" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DB9BC1E4-A720-4718-9573-7E995F300C41}" name="Notes + Weekly Total" dataDxfId="1" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A50C7FB5-E8D1-46A9-8CDE-3F2976E1126B}" name="Milestones" dataDxfId="0" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -743,7 +746,7 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -755,14 +758,14 @@
         <f>SUM(C3)</f>
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -774,7 +777,7 @@
       <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -786,7 +789,7 @@
       <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -798,7 +801,7 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -824,7 +827,7 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -836,7 +839,7 @@
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -848,7 +851,7 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
@@ -860,14 +863,14 @@
         <f>SUM(C6:C12)</f>
         <v>13</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -879,7 +882,7 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -891,7 +894,7 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -903,7 +906,7 @@
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -915,7 +918,7 @@
       <c r="C18" s="1">
         <v>0.5</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -927,7 +930,7 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -939,7 +942,7 @@
       <c r="C20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -954,7 +957,7 @@
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
@@ -966,14 +969,14 @@
         <f>SUM(C15:C21)</f>
         <v>5.5</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -985,7 +988,7 @@
       <c r="C24" s="1">
         <v>2</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -997,7 +1000,7 @@
       <c r="C25" s="1">
         <v>2.5</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1009,7 +1012,7 @@
       <c r="C26" s="1">
         <v>1.5</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -1021,7 +1024,7 @@
       <c r="C27" s="1">
         <v>2.5</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1033,7 +1036,7 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1045,7 +1048,7 @@
       <c r="C29" s="1">
         <v>1.5</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1057,7 +1060,7 @@
       <c r="C30" s="1">
         <v>2</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
@@ -1069,14 +1072,14 @@
         <f>SUM(C24:C30)</f>
         <v>13</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1088,7 +1091,7 @@
       <c r="C33" s="1">
         <v>1.5</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
@@ -1100,7 +1103,7 @@
       <c r="C34" s="1">
         <v>3</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
@@ -1112,7 +1115,7 @@
       <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -1127,7 +1130,7 @@
       <c r="D36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -1142,7 +1145,7 @@
       <c r="D37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -1154,7 +1157,7 @@
       <c r="C38" s="1">
         <v>2.5</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -1166,7 +1169,7 @@
       <c r="C39" s="1">
         <v>2</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
@@ -1178,7 +1181,7 @@
         <f>SUM(C33:C39)</f>
         <v>15.5</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
@@ -1187,7 +1190,7 @@
       <c r="B41" s="3"/>
       <c r="C41" s="1"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="1"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1202,7 +1205,7 @@
       <c r="D42" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1219,7 +1222,7 @@
       <c r="D43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -1234,7 +1237,7 @@
       <c r="D44" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -1249,7 +1252,7 @@
       <c r="D45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -1264,7 +1267,7 @@
       <c r="D46" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
@@ -1279,7 +1282,7 @@
       <c r="D47" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="1"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -1294,7 +1297,7 @@
       <c r="D48" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
@@ -1306,7 +1309,7 @@
         <f>SUM(C42:C48)</f>
         <v>17</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -1315,7 +1318,7 @@
       <c r="B50" s="3"/>
       <c r="C50" s="1"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="1"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -1330,7 +1333,7 @@
       <c r="D51" s="2">
         <v>2.19</v>
       </c>
-      <c r="E51" s="1"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
@@ -1345,7 +1348,7 @@
       <c r="D52" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="1"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -1360,7 +1363,7 @@
       <c r="D53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="1"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -1375,7 +1378,7 @@
       <c r="D54" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="1"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -1390,7 +1393,7 @@
       <c r="D55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="1"/>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -1405,7 +1408,7 @@
       <c r="D56" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="1"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -1420,7 +1423,7 @@
       <c r="D57" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E57" s="1"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
@@ -1432,7 +1435,7 @@
         <f>SUM(C51:C57)</f>
         <v>10.65</v>
       </c>
-      <c r="E58" s="1"/>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -1441,7 +1444,7 @@
       <c r="B59" s="3"/>
       <c r="C59" s="1"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="1"/>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -1456,7 +1459,7 @@
       <c r="D60" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E60" s="1"/>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -1471,7 +1474,7 @@
       <c r="D61" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E61" s="1"/>
+      <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -1486,7 +1489,7 @@
       <c r="D62" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="1"/>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
@@ -1501,7 +1504,7 @@
       <c r="D63" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E63" s="1"/>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -1516,7 +1519,7 @@
       <c r="D64" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E64" s="1"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -1531,7 +1534,7 @@
       <c r="D65" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
@@ -1546,7 +1549,7 @@
       <c r="D66" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
@@ -1558,7 +1561,7 @@
         <f>SUM(C60:C66)</f>
         <v>12.65</v>
       </c>
-      <c r="E67" s="1"/>
+      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
@@ -1567,7 +1570,7 @@
       <c r="B68" s="3"/>
       <c r="C68" s="1"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="1"/>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
@@ -1582,7 +1585,7 @@
       <c r="D69" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E69" s="1"/>
+      <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
@@ -1597,7 +1600,7 @@
       <c r="D70" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
@@ -1612,7 +1615,7 @@
       <c r="D71" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E71" s="1"/>
+      <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
@@ -1627,7 +1630,7 @@
       <c r="D72" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
@@ -1642,7 +1645,7 @@
       <c r="D73" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E73" s="1"/>
+      <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
@@ -1657,7 +1660,7 @@
       <c r="D74" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E74" s="1"/>
+      <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
@@ -1672,7 +1675,7 @@
       <c r="D75" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E75" s="1"/>
+      <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
@@ -1684,7 +1687,7 @@
         <f>SUM(C69:C75)</f>
         <v>7.25</v>
       </c>
-      <c r="E76" s="1"/>
+      <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
@@ -1693,7 +1696,7 @@
       <c r="B77" s="3"/>
       <c r="C77" s="1"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="1"/>
+      <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
@@ -1708,7 +1711,7 @@
       <c r="D78" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E78" s="1"/>
+      <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
@@ -1723,7 +1726,7 @@
       <c r="D79" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E79" s="1"/>
+      <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
@@ -1738,7 +1741,7 @@
       <c r="D80" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
@@ -1753,7 +1756,7 @@
       <c r="D81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E81" s="1"/>
+      <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
@@ -1768,7 +1771,7 @@
       <c r="D82" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E82" s="1"/>
+      <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
@@ -1783,7 +1786,7 @@
       <c r="D83" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E83" s="1"/>
+      <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
@@ -1798,7 +1801,7 @@
       <c r="D84" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1812,7 +1815,7 @@
         <f>SUM(C78:C84)</f>
         <v>11.25</v>
       </c>
-      <c r="E85" s="1"/>
+      <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
@@ -1821,7 +1824,7 @@
       <c r="B86" s="3"/>
       <c r="C86" s="1"/>
       <c r="D86" s="3"/>
-      <c r="E86" s="1"/>
+      <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
@@ -1836,7 +1839,7 @@
       <c r="D87" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E87" s="1"/>
+      <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
@@ -1851,7 +1854,7 @@
       <c r="D88" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E88" s="1"/>
+      <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
@@ -1866,7 +1869,7 @@
       <c r="D89" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E89" s="1"/>
+      <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
@@ -1881,7 +1884,7 @@
       <c r="D90" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E90" s="1"/>
+      <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
@@ -1896,7 +1899,7 @@
       <c r="D91" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1913,7 +1916,7 @@
       <c r="D92" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E92" s="1"/>
+      <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
@@ -1928,7 +1931,7 @@
       <c r="D93" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E93" s="1"/>
+      <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
@@ -1940,7 +1943,7 @@
         <f>SUM(C87:C93)</f>
         <v>13.25</v>
       </c>
-      <c r="E94" s="1"/>
+      <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
@@ -1949,7 +1952,7 @@
       <c r="B95" s="3"/>
       <c r="C95" s="1"/>
       <c r="D95" s="3"/>
-      <c r="E95" s="1"/>
+      <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
@@ -1964,7 +1967,7 @@
       <c r="D96" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1981,7 +1984,7 @@
       <c r="D97" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E97" s="1"/>
+      <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
@@ -1996,7 +1999,7 @@
       <c r="D98" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E98" s="1"/>
+      <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
@@ -2011,7 +2014,7 @@
       <c r="D99" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E99" s="1"/>
+      <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
@@ -2026,7 +2029,7 @@
       <c r="D100" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E100" s="1"/>
+      <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
@@ -2041,7 +2044,7 @@
       <c r="D101" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E101" s="1"/>
+      <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
@@ -2056,7 +2059,7 @@
       <c r="D102" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E102" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2070,7 +2073,7 @@
         <f>SUM(C96:C102)</f>
         <v>12</v>
       </c>
-      <c r="E103" s="1"/>
+      <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
@@ -2078,7 +2081,7 @@
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="1"/>
+      <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
@@ -2093,7 +2096,7 @@
       <c r="D105" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E105" s="1"/>
+      <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
@@ -2108,7 +2111,7 @@
       <c r="D106" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="1"/>
+      <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
@@ -2123,7 +2126,7 @@
       <c r="D107" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E107" s="1"/>
+      <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
@@ -2138,7 +2141,7 @@
       <c r="D108" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E108" s="1"/>
+      <c r="E108" s="2"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
@@ -2153,7 +2156,7 @@
       <c r="D109" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E109" s="1"/>
+      <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
@@ -2168,7 +2171,7 @@
       <c r="D110" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E110" s="1"/>
+      <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
@@ -2183,7 +2186,7 @@
       <c r="D111" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E111" s="1"/>
+      <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
@@ -2195,14 +2198,14 @@
         <f>SUM(C105:C111)</f>
         <v>8.75</v>
       </c>
-      <c r="E112" s="1"/>
+      <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
@@ -2217,7 +2220,7 @@
       <c r="D114" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E114" s="1"/>
+      <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
@@ -2232,7 +2235,7 @@
       <c r="D115" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E115" s="1"/>
+      <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
@@ -2247,7 +2250,7 @@
       <c r="D116" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E116" s="1"/>
+      <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
@@ -2262,7 +2265,7 @@
       <c r="D117" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E117" s="1"/>
+      <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
@@ -2277,7 +2280,7 @@
       <c r="D118" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E118" s="2" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2294,7 +2297,7 @@
       <c r="D119" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E119" s="1"/>
+      <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
@@ -2309,7 +2312,7 @@
       <c r="D120" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E120" s="1"/>
+      <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
@@ -2321,14 +2324,14 @@
         <f>SUM(C114:C120)</f>
         <v>14.75</v>
       </c>
-      <c r="E121" s="1"/>
+      <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C122" s="1"/>
-      <c r="E122" s="1"/>
+      <c r="E122" s="2"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
@@ -2338,54 +2341,56 @@
         <v>17</v>
       </c>
       <c r="C123" s="1">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E123" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>44543</v>
       </c>
       <c r="C124" s="1"/>
-      <c r="E124" s="1"/>
+      <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>44544</v>
       </c>
       <c r="C125" s="1"/>
-      <c r="E125" s="1"/>
+      <c r="E125" s="2"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>44545</v>
       </c>
       <c r="C126" s="1"/>
-      <c r="E126" s="1"/>
+      <c r="E126" s="2"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>44546</v>
       </c>
       <c r="C127" s="1"/>
-      <c r="E127" s="1"/>
+      <c r="E127" s="2"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>44547</v>
       </c>
       <c r="C128" s="1"/>
-      <c r="E128" s="1"/>
+      <c r="E128" s="2"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>44548</v>
       </c>
       <c r="C129" s="1"/>
-      <c r="E129" s="1"/>
+      <c r="E129" s="2"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
@@ -2395,9 +2400,9 @@
       <c r="C130" s="1"/>
       <c r="D130" s="3">
         <f>SUM(C123:C129)</f>
-        <v>0.75</v>
-      </c>
-      <c r="E130" s="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="E130" s="2"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
@@ -2405,7 +2410,7 @@
       </c>
       <c r="C131" s="1">
         <f>SUBTOTAL(109,Table1[Hours])</f>
-        <v>157.30000000000001</v>
+        <v>157.80000000000001</v>
       </c>
       <c r="E131" s="2"/>
     </row>

</xml_diff>